<commit_message>
Continuamos mañana, P2 ANSYS
</commit_message>
<xml_diff>
--- a/P2_lag_files/cuentas.xlsx
+++ b/P2_lag_files/cuentas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismael.llamas\Documents\GitHub\EYSTDUN_23-24\P2_lag_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\OneDrive - Universidad de Alcala\Escritorio\UNI\GitHub\EYSTDUN_23-24\P2_lag_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6E313C6-E986-42AF-B1DB-162BAAE6D902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0383124-C7D2-452A-8725-2CA2E09EE1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8F17334-E1C6-499D-A172-6FC81392E163}"/>
+    <workbookView xWindow="28695" yWindow="75" windowWidth="14610" windowHeight="15585" xr2:uid="{E8F17334-E1C6-499D-A172-6FC81392E163}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -84,6 +84,39 @@
   </si>
   <si>
     <t>Amplitud 2</t>
+  </si>
+  <si>
+    <t>Empotramiento A</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>1º max contado</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Da igual, es un factor arriba y abajo</t>
+  </si>
+  <si>
+    <t>Empotramiento B</t>
   </si>
 </sst>
 </file>
@@ -107,12 +140,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,10 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,10 +189,1066 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>fn(L)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>380</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.1700042873286156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0242154889775827</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3451680349198902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5883582110709487</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-496A-4A97-AA52-7EA4629D87EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="642060624"/>
+        <c:axId val="642068304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="642060624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>L (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="642068304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="642068304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>fn (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="642060624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>105727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3611C6CE-78C9-E745-E744-2E755F1AE424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,7 +1286,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -295,7 +1392,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -437,7 +1534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -445,15 +1542,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C385A7-27E4-4511-9601-BE79CEC42A00}">
-  <dimension ref="A3:J13"/>
+  <dimension ref="A3:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -482,7 +1582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -504,14 +1604,22 @@
         <f>1/E4</f>
         <v>3.0211480362537761</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>21.22</v>
       </c>
       <c r="H4">
         <v>14.95</v>
       </c>
+      <c r="I4">
+        <f>LOG((G4/H4))/10</f>
+        <v>1.5210418690487341E-2</v>
+      </c>
+      <c r="J4">
+        <f>I4/(SQRT(4*(PI()^2)+I4^2))</f>
+        <v>2.420806227728489E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -539,8 +1647,16 @@
       <c r="H5">
         <v>23.39</v>
       </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I7" si="1">LOG((G5/H5))/10</f>
+        <v>1.1583881091124933E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J7" si="2">I5/(SQRT(4*(PI()^2)+I5^2))</f>
+        <v>1.8436288026164047E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -568,8 +1684,16 @@
       <c r="H6">
         <v>33.119999999999997</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1.1458842406583975E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>1.8237283782645088E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -597,8 +1721,16 @@
       <c r="H7">
         <v>43.12</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.7420711518112985E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>2.7725816935163408E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -612,7 +1744,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -623,7 +1755,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -634,13 +1766,288 @@
         <v>5.3449999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13">
         <v>7.5880000000000001</v>
       </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.6</v>
+      </c>
+      <c r="B19">
+        <v>0.64470000000000005</v>
+      </c>
+      <c r="C19">
+        <v>3.9537</v>
+      </c>
+      <c r="D19">
+        <f>10/(C19-B19)</f>
+        <v>3.0220610456331216</v>
+      </c>
+      <c r="E19">
+        <v>22.821000000000002</v>
+      </c>
+      <c r="F19">
+        <v>15.8729</v>
+      </c>
+      <c r="G19">
+        <f>E19/(D19^2)</f>
+        <v>2.4987810590100001</v>
+      </c>
+      <c r="H19">
+        <f>F19/(D19^2)</f>
+        <v>1.7380001696489999</v>
+      </c>
+      <c r="I19">
+        <f>LOG((G19/H19))/10</f>
+        <v>1.5767839078955313E-2</v>
+      </c>
+      <c r="J19">
+        <f>I19/(SQRT(4*(PI()^2)+I19^2))</f>
+        <v>2.5095216291502872E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>19.079499999999999</v>
+      </c>
+      <c r="C20">
+        <v>22.364899999999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D21" si="3">10/(C20-B20)</f>
+        <v>3.0437694040299514</v>
+      </c>
+      <c r="E20">
+        <v>5.7634999999999996</v>
+      </c>
+      <c r="F20">
+        <v>4.5888999999999998</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G21" si="4">E20/(D20^2)</f>
+        <v>0.62210372687659965</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H21" si="5">F20/(D20^2)</f>
+        <v>0.49531912765923969</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20:I21" si="6">LOG((G20/H20))/10</f>
+        <v>9.8977703719624159E-3</v>
+      </c>
+      <c r="J20">
+        <f>I20/(SQRT(4*(PI()^2)+I20^2))</f>
+        <v>1.5752771257591517E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>36.1663</v>
+      </c>
+      <c r="C21">
+        <v>39.456400000000002</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>3.0394212941855847</v>
+      </c>
+      <c r="E21">
+        <v>2.4238</v>
+      </c>
+      <c r="F21">
+        <v>1.9384999999999999</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0.26237048464638041</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>0.20983793402385029</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>9.7030975794639655E-3</v>
+      </c>
+      <c r="J21">
+        <f>I21/(SQRT(4*(PI()^2)+I21^2))</f>
+        <v>1.5442941016209296E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.9</v>
+      </c>
+      <c r="B28">
+        <v>0.95440000000000003</v>
+      </c>
+      <c r="C28">
+        <v>3.5470999999999999</v>
+      </c>
+      <c r="D28">
+        <f>10/(C28-B28)</f>
+        <v>3.8569830678443324</v>
+      </c>
+      <c r="E28">
+        <v>29.652699999999999</v>
+      </c>
+      <c r="F28">
+        <v>22.558399999999999</v>
+      </c>
+      <c r="G28">
+        <f>LOG((E28/F28))/10</f>
+        <v>1.1875595060328032E-2</v>
+      </c>
+      <c r="H28">
+        <f>G28/(SQRT(4*(PI()^2)+G28^2))</f>
+        <v>1.8900562800637905E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>14.115500000000001</v>
+      </c>
+      <c r="C29">
+        <v>16.698599999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D30" si="7">10/(C29-B29)</f>
+        <v>3.8713174093143925</v>
+      </c>
+      <c r="E29">
+        <v>8.9047000000000001</v>
+      </c>
+      <c r="F29">
+        <v>6.8079999999999998</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G30" si="8">LOG((E29/F29))/10</f>
+        <v>1.1659974555605392E-2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H30" si="9">G29/(SQRT(4*(PI()^2)+G29^2))</f>
+        <v>1.8557393914734651E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>26.4468</v>
+      </c>
+      <c r="C30">
+        <v>29.006399999999999</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="7"/>
+        <v>3.9068604469448358</v>
+      </c>
+      <c r="E30">
+        <v>4.0358000000000001</v>
+      </c>
+      <c r="F30">
+        <v>3.3986000000000001</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>7.4629582921660565E-3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="9"/>
+        <v>1.1877658644432257E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>